<commit_message>
went through the papers to identify potential data to scrape
</commit_message>
<xml_diff>
--- a/data/classicalrefs.xlsx
+++ b/data/classicalrefs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzie/Documents/git/projects/grephon/grephon/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/britanywuuu/Documents/ubc/TemporalEcologyLab/grephon/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E4ABE5-6B92-7640-B896-9F9C92E5FB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285C9AD4-2E47-2B4A-B259-C5FC360C2DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="4420" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{EE02C19C-B795-5546-B78D-EEA02B5A84B7}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{EE02C19C-B795-5546-B78D-EEA02B5A84B7}"/>
   </bookViews>
   <sheets>
     <sheet name="dataoverview" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="136">
   <si>
     <t>growth_type</t>
   </si>
@@ -207,12 +207,261 @@
   <si>
     <t>By Lizzie so far</t>
   </si>
+  <si>
+    <t>https://doi.org/10.1111/j.1365-2486.2009.01990.x</t>
+  </si>
+  <si>
+    <t>huang2010</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/abs/10.1111/jbi.12462</t>
+  </si>
+  <si>
+    <t>dario2015</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/10.1111/gcb.16313</t>
+  </si>
+  <si>
+    <t>gantois2022</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s00442-013-2696-6</t>
+  </si>
+  <si>
+    <t>king2013</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/abs/10.1111/gcb.15170</t>
+  </si>
+  <si>
+    <t>klesse2020</t>
+  </si>
+  <si>
+    <t>https://www.jstor.org/stable/2390440</t>
+  </si>
+  <si>
+    <t>oleksyn1998</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/232697849_Intra-_and_interspecific_tree_growth_across_a_long_altitudinal_gradient_in_the_Peruvian_Andes</t>
+  </si>
+  <si>
+    <t>repp2012</t>
+  </si>
+  <si>
+    <t>https://www.jstor.org/stable/4496061</t>
+  </si>
+  <si>
+    <t>coomes2007</t>
+  </si>
+  <si>
+    <t>moser2009</t>
+  </si>
+  <si>
+    <t>no link found</t>
+  </si>
+  <si>
+    <t>https://besjournals.onlinelibrary.wiley.com/doi/full/10.1111/1365-2745.13603</t>
+  </si>
+  <si>
+    <t>hikosaka2021</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/geb.12245</t>
+  </si>
+  <si>
+    <t>gillman2014</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/235428344_Site-and_species-specific_responses_of_forest_growth_to_climate_across_the_European_continent</t>
+  </si>
+  <si>
+    <t>babst2013</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.dendro.2021.125914</t>
+  </si>
+  <si>
+    <t>zhou2022</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41598-018-37823-w</t>
+  </si>
+  <si>
+    <t>liang2019</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/978-1-4612-2178-4_39</t>
+  </si>
+  <si>
+    <t>cook1998</t>
+  </si>
+  <si>
+    <t>https://bioone.org/journals/tree-ring-research/volume-65/issue-2/2008-17.1/Climate-Radial-Growth-Relationships-of-Northern-Latitudinal-Range-Margin-Longleaf/10.3959/2008-17.1.full</t>
+  </si>
+  <si>
+    <t>bhuta2009</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/gcb.13366</t>
+  </si>
+  <si>
+    <t>cavin2016</t>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/full/10.1029/2017JG004292</t>
+  </si>
+  <si>
+    <t>zhu2018</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>Populus tremuloides, Betula papyrifera, Picea mariana, and Pinus banksiana</t>
+  </si>
+  <si>
+    <t>Quercus alba L. and Quercus montana Willd., Quercus rubra L. and Quercus velutina Lam., Carya glabra (Mill.) Sweet, Carya ovata (Mill.) K.Koch, Liriodendron tulipifera L., Acer rubrum L.</t>
+  </si>
+  <si>
+    <t>doesn't have raw data</t>
+  </si>
+  <si>
+    <t>has mean tree ring width but figures use tree ring indices which is tree ring width standardized with spline function. Compared with latitude not elevation (mostly 300-400 m flat topography)</t>
+  </si>
+  <si>
+    <t>Larix decidua, Picea abies</t>
+  </si>
+  <si>
+    <t>deciduous ! Only correlation between tree ring width and mean monthly climate. Appendix has chronology but no raw tree ring data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">has raw tree ring data but in the form of line plots </t>
+  </si>
+  <si>
+    <t>fig 3 could be scraped?</t>
+  </si>
+  <si>
+    <t>Pseudotsuga menziesii</t>
+  </si>
+  <si>
+    <t>Tree ring width</t>
+  </si>
+  <si>
+    <t>data from paleo data search</t>
+  </si>
+  <si>
+    <t>climatic data</t>
+  </si>
+  <si>
+    <t>Picea abies</t>
+  </si>
+  <si>
+    <t>altitude</t>
+  </si>
+  <si>
+    <t>DBH increment and height increment</t>
+  </si>
+  <si>
+    <t>Weinmannia lechleriana, W. pinnata, W. ovata, W. multijuga, W. reticulata, W. bangii, W. mariquitae, W. crassifolia, W. microphylla</t>
+  </si>
+  <si>
+    <t>mean diameter increment</t>
+  </si>
+  <si>
+    <t>might be hard to scrape (overlapping points)</t>
+  </si>
+  <si>
+    <t>Nothofagus solandri var. cliffortioides</t>
+  </si>
+  <si>
+    <t>used model to estimate growth</t>
+  </si>
+  <si>
+    <t>Fagus crenata, Abies mariesii</t>
+  </si>
+  <si>
+    <t>leaf basal area</t>
+  </si>
+  <si>
+    <t>table 1 and fig 2</t>
+  </si>
+  <si>
+    <t>do we want leaf basal area?</t>
+  </si>
+  <si>
+    <t>NPP</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>NPP of the whole forest</t>
+  </si>
+  <si>
+    <t>Picea abies, Pinus sylvestris, Abies alba, Larix decidua, Pinus cembra, Fagus sylvatica, Quercus robur, Quercus petraea</t>
+  </si>
+  <si>
+    <t>correlation, need to find raw data</t>
+  </si>
+  <si>
+    <t>data in suppliment files</t>
+  </si>
+  <si>
+    <t>Pinus yunnanensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fig 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betula ermanii, Picea jezoensis, Abies nephrolepis, Larix olgensis, Pinus koraiensis, Betula platyphylla, Pinus koraiensis, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean sensitivity </t>
+  </si>
+  <si>
+    <t>only has mean sensitivity</t>
+  </si>
+  <si>
+    <t>Pinus taeda L., P. elliottii Engelm. var. elliottii, P. paiustris Mill., P. echinata Mill.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year </t>
+  </si>
+  <si>
+    <t xml:space="preserve">no elevation info </t>
+  </si>
+  <si>
+    <t>Pinus palustris P. Mill.</t>
+  </si>
+  <si>
+    <t>both at 12 m asl</t>
+  </si>
+  <si>
+    <t>Fagus sylvatica L.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tree ring indices </t>
+  </si>
+  <si>
+    <t>line plots, basal area increment box plots available in supporting info, mean diameter of each site in supporting info</t>
+  </si>
+  <si>
+    <t>data in supporting info file</t>
+  </si>
+  <si>
+    <t>Tree ring width increment</t>
+  </si>
+  <si>
+    <t>Phellodendron amurense</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,6 +490,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -263,11 +518,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -583,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771102EB-8518-CC46-9A43-E451342C498E}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,10 +927,432 @@
         <v>47</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://link.springer.com/article/10.1007/BF00140166" xr:uid="{3590FF25-A9AF-354F-92FD-2E90587DFB60}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{2CD7E6F7-47A5-ED42-9091-C3EC721B14F4}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{C0399705-1E31-EF44-9499-AEF9568733F5}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{30AAA3AA-A794-224E-9122-96900550489A}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{6EEC3F9A-183B-7D43-AD3C-476C0B336ABF}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{2B217CA3-E33A-4147-A811-9572BA4A58B3}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{729698E3-0C65-2345-8D39-42D9921470D8}"/>
+    <hyperlink ref="A13" r:id="rId8" xr:uid="{A0212FDC-256A-F345-9036-02485FFDCA28}"/>
+    <hyperlink ref="A16" r:id="rId9" xr:uid="{61E9A40B-470F-604E-9406-08C1B2CB4831}"/>
+    <hyperlink ref="A17" r:id="rId10" xr:uid="{46170447-B373-6247-9188-6FFFC375E9EC}"/>
+    <hyperlink ref="A9" r:id="rId11" xr:uid="{A95B3B7E-D800-7746-8234-D8A709C30A51}"/>
+    <hyperlink ref="A10" r:id="rId12" xr:uid="{E51E0E70-6C3D-2C44-A341-41C170229795}"/>
+    <hyperlink ref="A11" r:id="rId13" xr:uid="{BBCDEF1C-C6E9-1E4F-AE27-029E41678B69}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{6CB239FA-3E0F-E14F-93BB-2BE5CF83E094}"/>
+    <hyperlink ref="A18" r:id="rId15" xr:uid="{ECAFEA9D-50E0-6B45-A22E-5EE596CD93F5}"/>
+    <hyperlink ref="A19" r:id="rId16" xr:uid="{60021276-6C1C-274A-90B3-3AFCDF1EE20A}"/>
+    <hyperlink ref="A20" r:id="rId17" xr:uid="{2927A3AA-9669-CD43-84F7-B1EE5406C191}"/>
+    <hyperlink ref="A21" r:id="rId18" xr:uid="{124C237A-95DE-DA44-8F1B-C9C291762803}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -680,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7738025-011D-C045-9941-7CF971814238}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -724,6 +1404,11 @@
       </c>
       <c r="L1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -735,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3E0F1A-F6C8-AC46-B6CF-939E66C1A554}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated wang2017 measurement unit (tree ring width)
</commit_message>
<xml_diff>
--- a/data/classicalrefs.xlsx
+++ b/data/classicalrefs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/britanywuuu/Documents/ubc/TemporalEcologyLab/grephon/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/britanywuuu/Documents/ubc/year5/TemporalEcologyLab/grephon/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A8779C-DF1C-1342-BD88-7445B8706AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0C2DE5-6386-5A4D-91B2-1B626E4CDC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" activeTab="1" xr2:uid="{EE02C19C-B795-5546-B78D-EEA02B5A84B7}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" xr2:uid="{EE02C19C-B795-5546-B78D-EEA02B5A84B7}"/>
   </bookViews>
   <sheets>
     <sheet name="dataoverview" sheetId="1" r:id="rId1"/>
@@ -679,9 +679,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -719,7 +719,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -825,7 +825,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -967,7 +967,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -977,7 +977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771102EB-8518-CC46-9A43-E451342C498E}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1555,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7738025-011D-C045-9941-7CF971814238}">
   <dimension ref="A1:L1447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1607,7 +1607,7 @@
         <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
         <v>121</v>
@@ -1643,7 +1643,7 @@
         <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="D3" t="s">
         <v>121</v>
@@ -1679,7 +1679,7 @@
         <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="D4" t="s">
         <v>121</v>
@@ -1715,7 +1715,7 @@
         <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="D5" t="s">
         <v>121</v>

</xml_diff>

<commit_message>
fixed methods and figure
</commit_message>
<xml_diff>
--- a/data/classicalrefs.xlsx
+++ b/data/classicalrefs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/britanywuuu/Documents/ubc/year5/TemporalEcologyLab/grephon/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50FD628-F7AB-2E40-82B2-5C48F7661868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F879E29E-966F-5F45-91C6-6BA60FD920C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" xr2:uid="{EE02C19C-B795-5546-B78D-EEA02B5A84B7}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" activeTab="1" xr2:uid="{EE02C19C-B795-5546-B78D-EEA02B5A84B7}"/>
   </bookViews>
   <sheets>
     <sheet name="dataoverview" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1000,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771102EB-8518-CC46-9A43-E451342C498E}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1556,6 +1556,112 @@
       </c>
       <c r="I23" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B25" t="str" cm="1">
+        <f t="array" ref="B25:B45">_xlfn.UNIQUE(B2:B23)</f>
+        <v>cook1991</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B26" t="str">
+        <v>wang2017</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B27" t="str">
+        <v>huang2010</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B28" t="str">
+        <v>dario2015</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B29" t="str">
+        <v>gantois2022</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B30" t="str">
+        <v>king2013</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B31" t="str">
+        <v>klesse2020</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B32" t="str">
+        <v>oleksyn1998</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="str">
+        <v>repp2012</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="str">
+        <v>coomes2007</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" t="str">
+        <v>moser2009</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" t="str">
+        <v>hikosaka2021</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" t="str">
+        <v>gillman2014</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="str">
+        <v>babst2013</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" t="str">
+        <v>zhou2022</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" t="str">
+        <v>liang2019</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" t="str">
+        <v>cook1998</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" t="str">
+        <v>bhuta2009</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="str">
+        <v>cavin2016</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" t="str">
+        <v>zhu2018</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="str">
+        <v>desauvage2022</v>
       </c>
     </row>
   </sheetData>
@@ -1590,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7738025-011D-C045-9941-7CF971814238}">
   <dimension ref="A1:L1453"/>
   <sheetViews>
-    <sheetView topLeftCell="A1000" workbookViewId="0">
-      <selection activeCell="A1453" sqref="A1453"/>
+    <sheetView tabSelected="1" topLeftCell="A1370" workbookViewId="0">
+      <selection activeCell="F1012" sqref="F1012"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>